<commit_message>
audio update + game data tool range fix
</commit_message>
<xml_diff>
--- a/GameDataConfigTool/excels/Audio.xlsx
+++ b/GameDataConfigTool/excels/Audio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\UnityProjects\SynthMind\GameDataConfigTool\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SynthMind\GameDataConfigTool\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6831C784-6708-4AA1-B081-1D4508801122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4F9EB7-8DB9-44DB-B654-D947DC2EE638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="4245" windowWidth="15060" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -384,7 +387,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>